<commit_message>
fix: set logo in excel report (GTS-2525)
</commit_message>
<xml_diff>
--- a/apps/admin/resources/report-templates/orders.xlsx
+++ b/apps/admin/resources/report-templates/orders.xlsx
@@ -8,43 +8,6 @@
     <sheet name="Отчёт по заказам" sheetId="1" r:id="rId4"/>
   </sheets>
 </workbook>
-</file>
-
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Anvar Zaitov</author>
-  </authors>
-  <commentList>
-    <comment ref="B10" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Helvetica Neue"/>
-          </rPr>
-          <t>Anvar Zaitov:
-ФИО Администратора</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B11" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Helvetica Neue"/>
-          </rPr>
-          <t>Anvar Zaitov:
-период всех ЗАКАЗОВ с датой завершения (самой поздней услуги)
-То есть в этот отчёт должны попасть только те ЗАКАЗЫ которые завершаються в этом периоде.</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -78,7 +41,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -131,11 +94,6 @@
       <sz val="12"/>
       <color indexed="11"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
     </font>
     <font>
       <b val="1"/>
@@ -224,7 +182,7 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -250,110 +208,6 @@
     </indexedColors>
   </colors>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>211152</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>100886</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>869752</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>77339</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="6" name="Рисунок 3"/>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="211152" y="100886"/>
-          <a:ext cx="2195301" cy="1035634"/>
-          <a:chOff x="0" y="0"/>
-          <a:chExt cx="2195299" cy="1035634"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:sp>
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="4" name="Прямоугольник"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="0" y="0"/>
-            <a:ext cx="2195299" cy="1035635"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:srgbClr val="EDEDED"/>
-          </a:solidFill>
-          <a:ln w="12700" cap="flat">
-            <a:noFill/>
-            <a:miter lim="400000"/>
-          </a:ln>
-          <a:effectLst/>
-        </xdr:spPr>
-        <xdr:txBody>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:pic>
-        <xdr:nvPicPr>
-          <xdr:cNvPr id="5" name="image1.jpeg" descr="image1.jpeg"/>
-          <xdr:cNvPicPr>
-            <a:picLocks noChangeAspect="1"/>
-          </xdr:cNvPicPr>
-        </xdr:nvPicPr>
-        <xdr:blipFill>
-          <a:blip r:embed="rId1">
-            <a:extLst/>
-          </a:blip>
-          <a:srcRect l="0" t="20546" r="0" b="28524"/>
-          <a:stretch>
-            <a:fillRect/>
-          </a:stretch>
-        </xdr:blipFill>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="-1" y="0"/>
-            <a:ext cx="2195301" cy="1035633"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln w="88900" cap="sq">
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF"/>
-            </a:solidFill>
-            <a:prstDash val="solid"/>
-            <a:miter lim="800000"/>
-          </a:ln>
-          <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="50800" dist="18000" dir="5400000">
-              <a:srgbClr val="000000">
-                <a:alpha val="40000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </xdr:spPr>
-      </xdr:pic>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1636,7 +1490,5 @@
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>